<commit_message>
Finished through Extreme Comp
</commit_message>
<xml_diff>
--- a/Extreme Networks Comps Analysis.xlsx
+++ b/Extreme Networks Comps Analysis.xlsx
@@ -64,8 +64,130 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Mary Roberts</author>
+  </authors>
+  <commentList>
+    <comment ref="C71" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Q4 PR: stock based comp, restructuring charge, litigation, gain on sale of facility, ceo expense.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C72" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Q4 PR: Currency loss from closing foreign subsidiary.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C77" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>10-K CFS</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C103" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2014 Q2 PR:
+stock based comp, acquisition and integratoin, restructuring, amortization, purchase accounting.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C109" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">2014 Q2 CFS excluding amortization already adjusted in non-GAAP op expense
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C134" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2014 Q2 PR:
+stock based comp, restructuring charge, litigation settlement, gain on facility sale.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C135" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2014 Q2 PR: currency loss from closing foreign subsidiary.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C140" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2014 Q2 CFS</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="183">
   <si>
     <t>Comments</t>
   </si>
@@ -611,13 +733,16 @@
   </si>
   <si>
     <t>Q2</t>
+  </si>
+  <si>
+    <t>FactSet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="88">
+  <numFmts count="90">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
@@ -706,8 +831,10 @@
     <numFmt numFmtId="244" formatCode="#,##0.0_);[Red]\(#,##0.0\);&quot;--  &quot;"/>
     <numFmt numFmtId="245" formatCode="0.00\x"/>
     <numFmt numFmtId="246" formatCode="0.0&quot; years&quot;"/>
+    <numFmt numFmtId="251" formatCode="#,##0.000_);\(#,##0.000\);\-_);@_)"/>
+    <numFmt numFmtId="255" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="104">
+  <fonts count="106">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1379,6 +1506,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="41">
@@ -2319,7 +2459,7 @@
     <xf numFmtId="0" fontId="96" fillId="0" borderId="0" applyAlignment="0"/>
     <xf numFmtId="246" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="187">
+  <cellXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2629,6 +2769,16 @@
     <xf numFmtId="228" fontId="64" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="251" fontId="64" fillId="32" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="231" fontId="0" fillId="32" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="236" fontId="64" fillId="32" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="236" fontId="64" fillId="32" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="232" fontId="64" fillId="32" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="255" fontId="64" fillId="32" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="200" fontId="64" fillId="32" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="236" fontId="64" fillId="32" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="239" fontId="64" fillId="32" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="227" fontId="81" fillId="32" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="212">
     <cellStyle name="$" xfId="1"/>
@@ -2963,22 +3113,22 @@
                 <c:formatCode>"$"#,##0.00_);\("$"#,##0.00\);@_)</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>5.5599999999999987</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5.5599999999999987</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>5.5599999999999987</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>5.5599999999999987</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>5.5599999999999987</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>5.5599999999999987</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3166,22 +3316,22 @@
                 <c:formatCode>"$"#,##0.00_);\("$"#,##0.00\);@_)</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>5.5599999999999987</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5.5599999999999987</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>5.5599999999999987</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>5.5599999999999987</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>5.5599999999999987</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>5.5599999999999987</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4538,15 +4688,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z289"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="7" topLeftCell="C114" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C209" sqref="C209:L209"/>
       <selection pane="topRight" activeCell="C209" sqref="C209:L209"/>
       <selection pane="bottomLeft" activeCell="C209" sqref="C209:L209"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="F205" sqref="F205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -4842,7 +4992,9 @@
         <v>5</v>
       </c>
       <c r="B15" s="8"/>
-      <c r="C15" s="140"/>
+      <c r="C15" s="187">
+        <v>95.867419999999996</v>
+      </c>
       <c r="D15" s="141"/>
       <c r="E15" s="141"/>
       <c r="F15" s="141"/>
@@ -4874,7 +5026,9 @@
         <v>1</v>
       </c>
       <c r="B17" s="8"/>
-      <c r="C17" s="144"/>
+      <c r="C17" s="144">
+        <v>0.94899999999999995</v>
+      </c>
       <c r="D17" s="144"/>
       <c r="E17" s="144"/>
       <c r="F17" s="144"/>
@@ -4891,7 +5045,9 @@
         <v>2</v>
       </c>
       <c r="B18" s="8"/>
-      <c r="C18" s="144"/>
+      <c r="C18" s="144">
+        <v>3.1E-2</v>
+      </c>
       <c r="D18" s="144"/>
       <c r="E18" s="144"/>
       <c r="F18" s="144"/>
@@ -4908,7 +5064,9 @@
         <v>3</v>
       </c>
       <c r="B19" s="8"/>
-      <c r="C19" s="144"/>
+      <c r="C19" s="144">
+        <v>0.54600000000000004</v>
+      </c>
       <c r="D19" s="144"/>
       <c r="E19" s="144"/>
       <c r="F19" s="144"/>
@@ -4925,7 +5083,9 @@
         <v>4</v>
       </c>
       <c r="B20" s="8"/>
-      <c r="C20" s="144"/>
+      <c r="C20" s="144">
+        <v>0.39500000000000002</v>
+      </c>
       <c r="D20" s="144"/>
       <c r="E20" s="144"/>
       <c r="F20" s="144"/>
@@ -4942,7 +5102,9 @@
         <v>5</v>
       </c>
       <c r="B21" s="8"/>
-      <c r="C21" s="144"/>
+      <c r="C21" s="144">
+        <v>0.39400000000000002</v>
+      </c>
       <c r="D21" s="144"/>
       <c r="E21" s="144"/>
       <c r="F21" s="144"/>
@@ -4959,7 +5121,9 @@
         <v>6</v>
       </c>
       <c r="B22" s="8"/>
-      <c r="C22" s="144"/>
+      <c r="C22" s="144">
+        <v>0.90100000000000002</v>
+      </c>
       <c r="D22" s="144"/>
       <c r="E22" s="144"/>
       <c r="F22" s="144"/>
@@ -4976,7 +5140,9 @@
         <v>7</v>
       </c>
       <c r="B23" s="8"/>
-      <c r="C23" s="144"/>
+      <c r="C23" s="144">
+        <v>0.98599999999999999</v>
+      </c>
       <c r="D23" s="144"/>
       <c r="E23" s="144"/>
       <c r="F23" s="144"/>
@@ -4993,7 +5159,9 @@
         <v>8</v>
       </c>
       <c r="B24" s="8"/>
-      <c r="C24" s="144"/>
+      <c r="C24" s="144">
+        <v>0.58599999999999997</v>
+      </c>
       <c r="D24" s="144"/>
       <c r="E24" s="144"/>
       <c r="F24" s="144"/>
@@ -5010,7 +5178,9 @@
         <v>9</v>
       </c>
       <c r="B25" s="8"/>
-      <c r="C25" s="144"/>
+      <c r="C25" s="144">
+        <v>7.0000000000000001E-3</v>
+      </c>
       <c r="D25" s="144"/>
       <c r="E25" s="144"/>
       <c r="F25" s="144"/>
@@ -5027,7 +5197,9 @@
         <v>10</v>
       </c>
       <c r="B26" s="8"/>
-      <c r="C26" s="144"/>
+      <c r="C26" s="189">
+        <v>0.06</v>
+      </c>
       <c r="D26" s="144"/>
       <c r="E26" s="144"/>
       <c r="F26" s="144"/>
@@ -5111,7 +5283,7 @@
       <c r="B31" s="8"/>
       <c r="C31" s="60">
         <f>SUM(C17:C30)</f>
-        <v>0</v>
+        <v>4.8549999999999995</v>
       </c>
       <c r="D31" s="60">
         <f t="shared" ref="D31:L31" si="2">SUM(D17:D30)</f>
@@ -5171,7 +5343,9 @@
         <v>1</v>
       </c>
       <c r="B33" s="8"/>
-      <c r="C33" s="146"/>
+      <c r="C33" s="188">
+        <v>2.4500000000000002</v>
+      </c>
       <c r="D33" s="146"/>
       <c r="E33" s="146"/>
       <c r="F33" s="146"/>
@@ -5188,7 +5362,9 @@
         <v>2</v>
       </c>
       <c r="B34" s="8"/>
-      <c r="C34" s="146"/>
+      <c r="C34" s="188">
+        <v>3.17</v>
+      </c>
       <c r="D34" s="146"/>
       <c r="E34" s="146"/>
       <c r="F34" s="146"/>
@@ -5205,7 +5381,9 @@
         <v>3</v>
       </c>
       <c r="B35" s="8"/>
-      <c r="C35" s="146"/>
+      <c r="C35" s="188">
+        <v>3.33</v>
+      </c>
       <c r="D35" s="146"/>
       <c r="E35" s="146"/>
       <c r="F35" s="146"/>
@@ -5222,7 +5400,9 @@
         <v>4</v>
       </c>
       <c r="B36" s="8"/>
-      <c r="C36" s="146"/>
+      <c r="C36" s="188">
+        <v>3.53</v>
+      </c>
       <c r="D36" s="146"/>
       <c r="E36" s="146"/>
       <c r="F36" s="146"/>
@@ -5239,7 +5419,9 @@
         <v>5</v>
       </c>
       <c r="B37" s="8"/>
-      <c r="C37" s="146"/>
+      <c r="C37" s="188">
+        <v>3.64</v>
+      </c>
       <c r="D37" s="146"/>
       <c r="E37" s="146"/>
       <c r="F37" s="146"/>
@@ -5256,7 +5438,9 @@
         <v>6</v>
       </c>
       <c r="B38" s="8"/>
-      <c r="C38" s="146"/>
+      <c r="C38" s="188">
+        <v>3.85</v>
+      </c>
       <c r="D38" s="146"/>
       <c r="E38" s="146"/>
       <c r="F38" s="146"/>
@@ -5273,7 +5457,9 @@
         <v>7</v>
       </c>
       <c r="B39" s="8"/>
-      <c r="C39" s="146"/>
+      <c r="C39" s="188">
+        <v>4.3600000000000003</v>
+      </c>
       <c r="D39" s="146"/>
       <c r="E39" s="146"/>
       <c r="F39" s="146"/>
@@ -5290,7 +5476,9 @@
         <v>8</v>
       </c>
       <c r="B40" s="8"/>
-      <c r="C40" s="146"/>
+      <c r="C40" s="188">
+        <v>6.5</v>
+      </c>
       <c r="D40" s="146"/>
       <c r="E40" s="146"/>
       <c r="F40" s="146"/>
@@ -5307,7 +5495,9 @@
         <v>9</v>
       </c>
       <c r="B41" s="8"/>
-      <c r="C41" s="146"/>
+      <c r="C41" s="188">
+        <v>8.36</v>
+      </c>
       <c r="D41" s="146"/>
       <c r="E41" s="146"/>
       <c r="F41" s="146"/>
@@ -5324,7 +5514,9 @@
         <v>10</v>
       </c>
       <c r="B42" s="8"/>
-      <c r="C42" s="146"/>
+      <c r="C42" s="188">
+        <v>9.8000000000000007</v>
+      </c>
       <c r="D42" s="146"/>
       <c r="E42" s="146"/>
       <c r="F42" s="146"/>
@@ -5424,7 +5616,7 @@
       <c r="B48" s="8"/>
       <c r="C48" s="57">
         <f t="shared" ref="C48:L48" si="4">SUMPRODUCT((C33:C46&lt;C11)*(C33:C46),C17:C30)</f>
-        <v>0</v>
+        <v>14.837820000000001</v>
       </c>
       <c r="D48" s="57">
         <f t="shared" si="4"/>
@@ -5470,7 +5662,7 @@
       <c r="B49" s="8"/>
       <c r="C49" s="56">
         <f>SUMIF(C33:C46,"&lt;"&amp;C11,C17:C30)</f>
-        <v>0</v>
+        <v>4.202</v>
       </c>
       <c r="D49" s="56">
         <f t="shared" ref="D49:L49" si="5">SUMIF(D33:D46,"&lt;"&amp;D11,D17:D30)</f>
@@ -5516,7 +5708,7 @@
       <c r="B50" s="8"/>
       <c r="C50" s="114">
         <f>IFERROR(C49-C48/C11, 0)</f>
-        <v>0</v>
+        <v>1.5333273381294958</v>
       </c>
       <c r="D50" s="114">
         <f t="shared" ref="D50:L50" si="6">IFERROR(D49-D48/D11, 0)</f>
@@ -5594,7 +5786,7 @@
       <c r="B53" s="8"/>
       <c r="C53" s="115">
         <f t="shared" ref="C53:L53" si="7">C15+SUM(C50:C52)</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="D53" s="115">
         <f t="shared" si="7"/>
@@ -5756,7 +5948,9 @@
         <v>7</v>
       </c>
       <c r="B59" s="8"/>
-      <c r="C59" s="140"/>
+      <c r="C59" s="150">
+        <v>299.34299999999996</v>
+      </c>
       <c r="D59" s="140"/>
       <c r="E59" s="140"/>
       <c r="F59" s="140"/>
@@ -5771,7 +5965,10 @@
       <c r="A60" s="113" t="s">
         <v>87</v>
       </c>
-      <c r="C60" s="144"/>
+      <c r="C60" s="191">
+        <f>-136.717</f>
+        <v>-136.71700000000001</v>
+      </c>
       <c r="D60" s="144"/>
       <c r="E60" s="144"/>
       <c r="F60" s="144"/>
@@ -5791,11 +5988,11 @@
       </c>
       <c r="B61" s="8"/>
       <c r="C61" s="142">
-        <f t="shared" ref="C61:F61" si="10">SUM(C59:C60)</f>
-        <v>0</v>
+        <f>(SUM(C59:C60))</f>
+        <v>162.62599999999995</v>
       </c>
       <c r="D61" s="142">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="C61:F61" si="10">SUM(D59:D60)</f>
         <v>0</v>
       </c>
       <c r="E61" s="142">
@@ -5835,7 +6032,10 @@
       <c r="A62" s="54" t="s">
         <v>154</v>
       </c>
-      <c r="C62" s="144"/>
+      <c r="C62" s="191">
+        <f>-151.774</f>
+        <v>-151.774</v>
+      </c>
       <c r="D62" s="144"/>
       <c r="E62" s="144"/>
       <c r="F62" s="144"/>
@@ -5856,7 +6056,7 @@
       <c r="B63" s="9"/>
       <c r="C63" s="149">
         <f>SUM(C61:C62)</f>
-        <v>0</v>
+        <v>10.851999999999947</v>
       </c>
       <c r="D63" s="149">
         <f t="shared" ref="D63:F63" si="12">SUM(D61:D62)</f>
@@ -5902,7 +6102,10 @@
         <v>167</v>
       </c>
       <c r="B64" s="8"/>
-      <c r="C64" s="140"/>
+      <c r="C64" s="192">
+        <f>1.07-0.571</f>
+        <v>0.49900000000000011</v>
+      </c>
       <c r="D64" s="140"/>
       <c r="E64" s="140"/>
       <c r="F64" s="140"/>
@@ -5922,11 +6125,11 @@
       </c>
       <c r="B65" s="8"/>
       <c r="C65" s="142">
-        <f t="shared" ref="C65:F65" si="14">SUM(C63:C64)</f>
-        <v>0</v>
+        <f>(SUM(C63:C64))</f>
+        <v>11.350999999999948</v>
       </c>
       <c r="D65" s="142">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="C65:F65" si="14">SUM(D63:D64)</f>
         <v>0</v>
       </c>
       <c r="E65" s="142">
@@ -5967,7 +6170,9 @@
         <v>86</v>
       </c>
       <c r="B66" s="8"/>
-      <c r="C66" s="140"/>
+      <c r="C66" s="150">
+        <v>-1.6780000000000002</v>
+      </c>
       <c r="D66" s="140"/>
       <c r="E66" s="140"/>
       <c r="F66" s="140"/>
@@ -5987,11 +6192,11 @@
       </c>
       <c r="B67" s="8"/>
       <c r="C67" s="142">
-        <f t="shared" ref="C67:F67" si="16">SUM(C65:C66)</f>
-        <v>0</v>
+        <f>(((SUM(C65:C66))/10)/10)/10</f>
+        <v>9.6729999999999473E-3</v>
       </c>
       <c r="D67" s="142">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="C67:F67" si="16">SUM(D65:D66)</f>
         <v>0</v>
       </c>
       <c r="E67" s="142">
@@ -6032,7 +6237,9 @@
         <v>85</v>
       </c>
       <c r="B68" s="8"/>
-      <c r="C68" s="140"/>
+      <c r="C68" s="150">
+        <v>95.043999999999997</v>
+      </c>
       <c r="D68" s="140"/>
       <c r="E68" s="140"/>
       <c r="F68" s="140"/>
@@ -6078,7 +6285,10 @@
         <v>157</v>
       </c>
       <c r="B71" s="8"/>
-      <c r="C71" s="140"/>
+      <c r="C71" s="140">
+        <f>6.511+6.836+2.197-11.539+2.086</f>
+        <v>6.0910000000000011</v>
+      </c>
       <c r="D71" s="140"/>
       <c r="E71" s="140"/>
       <c r="F71" s="140"/>
@@ -6097,7 +6307,9 @@
         <v>158</v>
       </c>
       <c r="B72" s="8"/>
-      <c r="C72" s="140"/>
+      <c r="C72" s="140">
+        <v>0.46500000000000002</v>
+      </c>
       <c r="D72" s="140"/>
       <c r="E72" s="140"/>
       <c r="F72" s="140"/>
@@ -6164,7 +6376,7 @@
       <c r="B76" s="8"/>
       <c r="C76" s="152">
         <f t="shared" ref="C76:L76" si="18">C63+C71</f>
-        <v>0</v>
+        <v>16.942999999999948</v>
       </c>
       <c r="D76" s="152">
         <f t="shared" si="18"/>
@@ -6208,7 +6420,10 @@
         <v>10</v>
       </c>
       <c r="B77" s="8"/>
-      <c r="C77" s="140"/>
+      <c r="C77" s="190">
+        <f>4.543+1.488</f>
+        <v>6.0310000000000006</v>
+      </c>
       <c r="D77" s="140"/>
       <c r="E77" s="140"/>
       <c r="F77" s="140"/>
@@ -6230,7 +6445,7 @@
       <c r="B78" s="8"/>
       <c r="C78" s="152">
         <f t="shared" ref="C78:L78" si="19">C76+C77</f>
-        <v>0</v>
+        <v>22.973999999999947</v>
       </c>
       <c r="D78" s="152">
         <f t="shared" si="19"/>
@@ -6276,7 +6491,7 @@
       <c r="B79" s="8"/>
       <c r="C79" s="152">
         <f t="shared" ref="C79:L79" si="20">C65+C71+C72</f>
-        <v>0</v>
+        <v>17.90699999999995</v>
       </c>
       <c r="D79" s="152">
         <f t="shared" si="20"/>
@@ -6322,7 +6537,7 @@
       <c r="B80" s="8"/>
       <c r="C80" s="152">
         <f t="shared" ref="C80:L80" si="21">C66+C73</f>
-        <v>0</v>
+        <v>-1.6780000000000002</v>
       </c>
       <c r="D80" s="152">
         <f t="shared" si="21"/>
@@ -6368,7 +6583,7 @@
       <c r="B81" s="8"/>
       <c r="C81" s="152">
         <f>C79+C80</f>
-        <v>0</v>
+        <v>16.228999999999949</v>
       </c>
       <c r="D81" s="152">
         <f t="shared" ref="D81:L81" si="22">D79+D80</f>
@@ -6475,7 +6690,7 @@
       <c r="B86" s="8"/>
       <c r="C86" s="153">
         <f>IFERROR((C81+C84)/(C68+C85),0)</f>
-        <v>0</v>
+        <v>0.17075249358191943</v>
       </c>
       <c r="D86" s="153">
         <f t="shared" ref="D86:L86" si="23">IFERROR((D81+D84)/(D68+D85),0)</f>
@@ -6677,7 +6892,9 @@
         <v>7</v>
       </c>
       <c r="B91" s="8"/>
-      <c r="C91" s="140"/>
+      <c r="C91" s="150">
+        <v>222.49799999999999</v>
+      </c>
       <c r="D91" s="140"/>
       <c r="E91" s="140"/>
       <c r="F91" s="140"/>
@@ -6692,7 +6909,9 @@
       <c r="A92" s="113" t="s">
         <v>87</v>
       </c>
-      <c r="C92" s="140"/>
+      <c r="C92" s="150">
+        <v>-108.947</v>
+      </c>
       <c r="D92" s="140"/>
       <c r="E92" s="140"/>
       <c r="F92" s="140"/>
@@ -6710,7 +6929,7 @@
       <c r="B93" s="8"/>
       <c r="C93" s="142">
         <f t="shared" ref="C93" si="27">SUM(C91:C92)</f>
-        <v>0</v>
+        <v>113.55099999999999</v>
       </c>
       <c r="D93" s="142">
         <f t="shared" ref="D93:F93" si="28">SUM(D91:D92)</f>
@@ -6753,7 +6972,9 @@
       <c r="A94" s="54" t="s">
         <v>154</v>
       </c>
-      <c r="C94" s="140"/>
+      <c r="C94" s="150">
+        <v>-126.952</v>
+      </c>
       <c r="D94" s="140"/>
       <c r="E94" s="140"/>
       <c r="F94" s="140"/>
@@ -6771,7 +6992,7 @@
       <c r="B95" s="9"/>
       <c r="C95" s="149">
         <f t="shared" ref="C95:F95" si="30">SUM(C93:C94)</f>
-        <v>0</v>
+        <v>-13.40100000000001</v>
       </c>
       <c r="D95" s="149">
         <f t="shared" si="30"/>
@@ -6815,7 +7036,10 @@
         <v>167</v>
       </c>
       <c r="B96" s="8"/>
-      <c r="C96" s="140"/>
+      <c r="C96" s="150">
+        <f>0.447-0.524-1.192</f>
+        <v>-1.2689999999999999</v>
+      </c>
       <c r="D96" s="140"/>
       <c r="E96" s="140"/>
       <c r="F96" s="140"/>
@@ -6833,7 +7057,7 @@
       <c r="B97" s="8"/>
       <c r="C97" s="142">
         <f t="shared" ref="C97:F97" si="32">SUM(C95:C96)</f>
-        <v>0</v>
+        <v>-14.670000000000011</v>
       </c>
       <c r="D97" s="142">
         <f t="shared" si="32"/>
@@ -6877,7 +7101,9 @@
         <v>86</v>
       </c>
       <c r="B98" s="8"/>
-      <c r="C98" s="140"/>
+      <c r="C98" s="150">
+        <v>-1.3520000000000001</v>
+      </c>
       <c r="D98" s="140"/>
       <c r="E98" s="140"/>
       <c r="F98" s="140"/>
@@ -6895,7 +7121,7 @@
       <c r="B99" s="8"/>
       <c r="C99" s="142">
         <f t="shared" ref="C99:F99" si="34">SUM(C97:C98)</f>
-        <v>0</v>
+        <v>-16.022000000000009</v>
       </c>
       <c r="D99" s="142">
         <f t="shared" si="34"/>
@@ -6939,7 +7165,9 @@
         <v>85</v>
       </c>
       <c r="B100" s="8"/>
-      <c r="C100" s="140"/>
+      <c r="C100" s="150">
+        <v>94.638999999999996</v>
+      </c>
       <c r="D100" s="140"/>
       <c r="E100" s="140"/>
       <c r="F100" s="140"/>
@@ -6985,7 +7213,10 @@
         <v>157</v>
       </c>
       <c r="B103" s="8"/>
-      <c r="C103" s="140"/>
+      <c r="C103" s="140">
+        <f>5.033+12.382+0.505+6.472+11</f>
+        <v>35.391999999999996</v>
+      </c>
       <c r="D103" s="140"/>
       <c r="E103" s="140"/>
       <c r="F103" s="140"/>
@@ -7065,7 +7296,7 @@
       <c r="B108" s="8"/>
       <c r="C108" s="152">
         <f t="shared" ref="C108:L108" si="36">C95+C103</f>
-        <v>0</v>
+        <v>21.990999999999985</v>
       </c>
       <c r="D108" s="152">
         <f t="shared" si="36"/>
@@ -7109,7 +7340,10 @@
         <v>10</v>
       </c>
       <c r="B109" s="8"/>
-      <c r="C109" s="140"/>
+      <c r="C109" s="150">
+        <f>4.143+6.997-6.472</f>
+        <v>4.6680000000000001</v>
+      </c>
       <c r="D109" s="140"/>
       <c r="E109" s="140"/>
       <c r="F109" s="140"/>
@@ -7127,7 +7361,7 @@
       <c r="B110" s="8"/>
       <c r="C110" s="152">
         <f t="shared" ref="C110:L110" si="37">C108+C109</f>
-        <v>0</v>
+        <v>26.658999999999985</v>
       </c>
       <c r="D110" s="152">
         <f t="shared" si="37"/>
@@ -7173,7 +7407,7 @@
       <c r="B111" s="8"/>
       <c r="C111" s="152">
         <f t="shared" ref="C111:L111" si="38">C97+C103+C104</f>
-        <v>0</v>
+        <v>20.721999999999987</v>
       </c>
       <c r="D111" s="152">
         <f t="shared" si="38"/>
@@ -7219,7 +7453,7 @@
       <c r="B112" s="8"/>
       <c r="C112" s="152">
         <f t="shared" ref="C112:L112" si="39">C98+C105</f>
-        <v>0</v>
+        <v>-1.3520000000000001</v>
       </c>
       <c r="D112" s="152">
         <f t="shared" si="39"/>
@@ -7265,7 +7499,7 @@
       <c r="B113" s="8"/>
       <c r="C113" s="152">
         <f t="shared" ref="C113:L113" si="40">C111+C112</f>
-        <v>0</v>
+        <v>19.369999999999987</v>
       </c>
       <c r="D113" s="152">
         <f t="shared" si="40"/>
@@ -7354,7 +7588,10 @@
       <c r="A117" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="C117" s="140"/>
+      <c r="C117" s="193">
+        <f>97.023-C100</f>
+        <v>2.3840000000000003</v>
+      </c>
       <c r="D117" s="140"/>
       <c r="E117" s="140"/>
       <c r="F117" s="140"/>
@@ -7372,7 +7609,7 @@
       <c r="B118" s="8"/>
       <c r="C118" s="153">
         <f t="shared" ref="C118:L118" si="41">IFERROR((C113+C116)/(C100+C117),0)</f>
-        <v>0</v>
+        <v>0.19964338352761704</v>
       </c>
       <c r="D118" s="153">
         <f t="shared" si="41"/>
@@ -7518,7 +7755,9 @@
         <v>7</v>
       </c>
       <c r="B122" s="8"/>
-      <c r="C122" s="140"/>
+      <c r="C122" s="150">
+        <v>151.678</v>
+      </c>
       <c r="D122" s="140"/>
       <c r="E122" s="140"/>
       <c r="F122" s="140"/>
@@ -7533,7 +7772,10 @@
       <c r="A123" s="113" t="s">
         <v>87</v>
       </c>
-      <c r="C123" s="144"/>
+      <c r="C123" s="191">
+        <f>-70.964</f>
+        <v>-70.963999999999999</v>
+      </c>
       <c r="D123" s="144"/>
       <c r="E123" s="144"/>
       <c r="F123" s="144"/>
@@ -7551,7 +7793,7 @@
       <c r="B124" s="8"/>
       <c r="C124" s="142">
         <f t="shared" ref="C124" si="44">SUM(C122:C123)</f>
-        <v>0</v>
+        <v>80.713999999999999</v>
       </c>
       <c r="D124" s="142">
         <f t="shared" ref="D124:F124" si="45">SUM(D122:D123)</f>
@@ -7594,7 +7836,9 @@
       <c r="A125" s="54" t="s">
         <v>154</v>
       </c>
-      <c r="C125" s="144"/>
+      <c r="C125" s="191">
+        <v>-70.903000000000006</v>
+      </c>
       <c r="D125" s="144"/>
       <c r="E125" s="144"/>
       <c r="F125" s="144"/>
@@ -7612,7 +7856,7 @@
       <c r="B126" s="9"/>
       <c r="C126" s="149">
         <f t="shared" ref="C126:F126" si="47">SUM(C124:C125)</f>
-        <v>0</v>
+        <v>9.8109999999999928</v>
       </c>
       <c r="D126" s="149">
         <f t="shared" si="47"/>
@@ -7656,7 +7900,10 @@
         <v>167</v>
       </c>
       <c r="B127" s="8"/>
-      <c r="C127" s="140"/>
+      <c r="C127" s="150">
+        <f>0.531-0.001-0.649</f>
+        <v>-0.11899999999999999</v>
+      </c>
       <c r="D127" s="140"/>
       <c r="E127" s="140"/>
       <c r="F127" s="140"/>
@@ -7674,7 +7921,7 @@
       <c r="B128" s="8"/>
       <c r="C128" s="142">
         <f t="shared" ref="C128:F128" si="49">SUM(C126:C127)</f>
-        <v>0</v>
+        <v>9.6919999999999931</v>
       </c>
       <c r="D128" s="142">
         <f t="shared" si="49"/>
@@ -7718,7 +7965,9 @@
         <v>86</v>
       </c>
       <c r="B129" s="8"/>
-      <c r="C129" s="140"/>
+      <c r="C129" s="150">
+        <v>-0.98299999999999998</v>
+      </c>
       <c r="D129" s="140"/>
       <c r="E129" s="140"/>
       <c r="F129" s="140"/>
@@ -7736,7 +7985,7 @@
       <c r="B130" s="8"/>
       <c r="C130" s="142">
         <f t="shared" ref="C130:F130" si="51">SUM(C128:C129)</f>
-        <v>0</v>
+        <v>8.7089999999999925</v>
       </c>
       <c r="D130" s="142">
         <f t="shared" si="51"/>
@@ -7780,7 +8029,9 @@
         <v>85</v>
       </c>
       <c r="B131" s="8"/>
-      <c r="C131" s="140"/>
+      <c r="C131" s="150">
+        <v>95.513999999999996</v>
+      </c>
       <c r="D131" s="140"/>
       <c r="E131" s="140"/>
       <c r="F131" s="140"/>
@@ -7826,7 +8077,10 @@
         <v>157</v>
       </c>
       <c r="B134" s="8"/>
-      <c r="C134" s="140"/>
+      <c r="C134" s="150">
+        <f>3.784+5.167-0.421-11.539</f>
+        <v>-3.0089999999999986</v>
+      </c>
       <c r="D134" s="140"/>
       <c r="E134" s="140"/>
       <c r="F134" s="140"/>
@@ -7842,7 +8096,10 @@
         <v>158</v>
       </c>
       <c r="B135" s="8"/>
-      <c r="C135" s="140"/>
+      <c r="C135" s="150">
+        <f>0.465</f>
+        <v>0.46500000000000002</v>
+      </c>
       <c r="D135" s="140"/>
       <c r="E135" s="140"/>
       <c r="F135" s="140"/>
@@ -7904,9 +8161,9 @@
         <v>8</v>
       </c>
       <c r="B139" s="8"/>
-      <c r="C139" s="152">
+      <c r="C139" s="142">
         <f t="shared" ref="C139:L139" si="53">C126+C134</f>
-        <v>0</v>
+        <v>6.8019999999999943</v>
       </c>
       <c r="D139" s="152">
         <f t="shared" si="53"/>
@@ -7950,7 +8207,10 @@
         <v>10</v>
       </c>
       <c r="B140" s="8"/>
-      <c r="C140" s="140"/>
+      <c r="C140" s="150">
+        <f>2.292+0.801</f>
+        <v>3.093</v>
+      </c>
       <c r="D140" s="140"/>
       <c r="E140" s="140"/>
       <c r="F140" s="140"/>
@@ -7966,9 +8226,9 @@
         <v>9</v>
       </c>
       <c r="B141" s="8"/>
-      <c r="C141" s="152">
+      <c r="C141" s="142">
         <f t="shared" ref="C141:L141" si="54">C139+C140</f>
-        <v>0</v>
+        <v>9.8949999999999942</v>
       </c>
       <c r="D141" s="152">
         <f t="shared" si="54"/>
@@ -8012,9 +8272,9 @@
         <v>35</v>
       </c>
       <c r="B142" s="8"/>
-      <c r="C142" s="152">
+      <c r="C142" s="142">
         <f t="shared" ref="C142:L142" si="55">C128+C134+C135</f>
-        <v>0</v>
+        <v>7.1479999999999944</v>
       </c>
       <c r="D142" s="152">
         <f t="shared" si="55"/>
@@ -8058,9 +8318,9 @@
         <v>86</v>
       </c>
       <c r="B143" s="8"/>
-      <c r="C143" s="152">
+      <c r="C143" s="142">
         <f t="shared" ref="C143:L143" si="56">C129+C136</f>
-        <v>0</v>
+        <v>-0.98299999999999998</v>
       </c>
       <c r="D143" s="152">
         <f t="shared" si="56"/>
@@ -8104,9 +8364,9 @@
         <v>150</v>
       </c>
       <c r="B144" s="8"/>
-      <c r="C144" s="152">
+      <c r="C144" s="142">
         <f t="shared" ref="C144:L144" si="57">C142+C143</f>
-        <v>0</v>
+        <v>6.1649999999999947</v>
       </c>
       <c r="D144" s="152">
         <f t="shared" si="57"/>
@@ -8213,7 +8473,7 @@
       <c r="B149" s="8"/>
       <c r="C149" s="153">
         <f t="shared" ref="C149:L149" si="58">IFERROR((C144+C147)/(C131+C148),0)</f>
-        <v>0</v>
+        <v>6.4545511652741958E-2</v>
       </c>
       <c r="D149" s="153">
         <f t="shared" si="58"/>
@@ -8377,7 +8637,7 @@
       </c>
       <c r="C154" s="162">
         <f t="shared" ref="C154:L154" si="61">C59+C91-C122</f>
-        <v>0</v>
+        <v>370.1629999999999</v>
       </c>
       <c r="D154" s="162">
         <f t="shared" si="61"/>
@@ -8422,7 +8682,7 @@
       </c>
       <c r="C155" s="163">
         <f t="shared" ref="C155:L155" si="62">C78+C110-C141</f>
-        <v>0</v>
+        <v>39.737999999999936</v>
       </c>
       <c r="D155" s="163">
         <f t="shared" si="62"/>
@@ -8467,7 +8727,7 @@
       </c>
       <c r="C156" s="163">
         <f t="shared" ref="C156:L156" si="63">C76+C108-C139</f>
-        <v>0</v>
+        <v>32.131999999999941</v>
       </c>
       <c r="D156" s="163">
         <f t="shared" si="63"/>
@@ -8512,7 +8772,7 @@
       </c>
       <c r="C157" s="164">
         <f t="shared" ref="C157:L157" si="64">C86+C118-C149</f>
-        <v>0</v>
+        <v>0.3058503654567945</v>
       </c>
       <c r="D157" s="164">
         <f t="shared" si="64"/>
@@ -8674,7 +8934,7 @@
       </c>
       <c r="C162" s="165">
         <f t="shared" ref="C162:L162" si="67">C59</f>
-        <v>0</v>
+        <v>299.34299999999996</v>
       </c>
       <c r="D162" s="165">
         <f t="shared" si="67"/>
@@ -8719,7 +8979,7 @@
       </c>
       <c r="C163" s="163">
         <f>C78</f>
-        <v>0</v>
+        <v>22.973999999999947</v>
       </c>
       <c r="D163" s="163">
         <f t="shared" ref="D163:L163" si="68">D78</f>
@@ -8764,7 +9024,7 @@
       </c>
       <c r="C164" s="163">
         <f>C76</f>
-        <v>0</v>
+        <v>16.942999999999948</v>
       </c>
       <c r="D164" s="163">
         <f t="shared" ref="D164:L164" si="69">D76</f>
@@ -8809,7 +9069,7 @@
       </c>
       <c r="C165" s="166">
         <f>C86</f>
-        <v>0</v>
+        <v>0.17075249358191943</v>
       </c>
       <c r="D165" s="166">
         <f t="shared" ref="D165:L165" si="70">D86</f>
@@ -8937,7 +9197,9 @@
       <c r="A170" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C170" s="144"/>
+      <c r="C170" s="144">
+        <v>4.0629999999999997</v>
+      </c>
       <c r="D170" s="144"/>
       <c r="E170" s="144"/>
       <c r="F170" s="144"/>
@@ -8952,7 +9214,9 @@
       <c r="A171" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C171" s="144"/>
+      <c r="C171" s="144">
+        <v>95.125</v>
+      </c>
       <c r="D171" s="144"/>
       <c r="E171" s="144"/>
       <c r="F171" s="144"/>
@@ -8967,7 +9231,9 @@
       <c r="A172" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C172" s="144"/>
+      <c r="C172" s="189">
+        <v>0</v>
+      </c>
       <c r="D172" s="144"/>
       <c r="E172" s="144"/>
       <c r="F172" s="144"/>
@@ -8982,7 +9248,9 @@
       <c r="A173" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C173" s="145"/>
+      <c r="C173" s="194">
+        <v>0</v>
+      </c>
       <c r="D173" s="145"/>
       <c r="E173" s="145"/>
       <c r="F173" s="145"/>
@@ -8999,7 +9267,7 @@
       </c>
       <c r="C174" s="168">
         <f>SUM(C170:C173)</f>
-        <v>0</v>
+        <v>99.188000000000002</v>
       </c>
       <c r="D174" s="168">
         <f>SUM(D170:D173)</f>
@@ -9042,7 +9310,10 @@
       <c r="A175" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C175" s="144"/>
+      <c r="C175" s="191">
+        <f>-68.304-43.713</f>
+        <v>-112.017</v>
+      </c>
       <c r="D175" s="144"/>
       <c r="E175" s="144"/>
       <c r="F175" s="144"/>
@@ -9063,7 +9334,7 @@
       <c r="B176" s="29"/>
       <c r="C176" s="169">
         <f>SUM(C174:C175)</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="D176" s="169">
         <f>SUM(D174:D175)</f>
@@ -9252,7 +9523,9 @@
       <c r="A183" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="C183" s="140"/>
+      <c r="C183" s="140">
+        <v>530.5</v>
+      </c>
       <c r="D183" s="144"/>
       <c r="E183" s="144"/>
       <c r="F183" s="144"/>
@@ -9273,7 +9546,9 @@
       <c r="A184" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C184" s="144"/>
+      <c r="C184" s="144">
+        <v>55.8</v>
+      </c>
       <c r="D184" s="144"/>
       <c r="E184" s="144"/>
       <c r="F184" s="144"/>
@@ -9294,7 +9569,9 @@
       <c r="A185" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C185" s="144"/>
+      <c r="C185" s="144">
+        <v>34.5</v>
+      </c>
       <c r="D185" s="144"/>
       <c r="E185" s="144"/>
       <c r="F185" s="144"/>
@@ -9315,7 +9592,9 @@
       <c r="A186" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C186" s="144"/>
+      <c r="C186" s="195">
+        <v>0.28000000000000003</v>
+      </c>
       <c r="D186" s="144"/>
       <c r="E186" s="144"/>
       <c r="F186" s="144"/>
@@ -9337,7 +9616,9 @@
         <v>42</v>
       </c>
       <c r="B187" s="38"/>
-      <c r="C187" s="173"/>
+      <c r="C187" s="173" t="s">
+        <v>182</v>
+      </c>
       <c r="D187" s="173"/>
       <c r="E187" s="173"/>
       <c r="F187" s="173"/>
@@ -9469,7 +9750,9 @@
       <c r="A192" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="C192" s="140"/>
+      <c r="C192" s="140">
+        <v>663</v>
+      </c>
       <c r="D192" s="140"/>
       <c r="E192" s="140"/>
       <c r="F192" s="140"/>
@@ -9488,7 +9771,9 @@
       <c r="A193" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="C193" s="144"/>
+      <c r="C193" s="144">
+        <v>85.8</v>
+      </c>
       <c r="D193" s="144"/>
       <c r="E193" s="144"/>
       <c r="F193" s="144"/>
@@ -9507,7 +9792,9 @@
       <c r="A194" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="C194" s="144"/>
+      <c r="C194" s="144">
+        <v>63.8</v>
+      </c>
       <c r="D194" s="144"/>
       <c r="E194" s="144"/>
       <c r="F194" s="144"/>
@@ -9526,7 +9813,9 @@
       <c r="A195" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="C195" s="144"/>
+      <c r="C195" s="195">
+        <v>0.56999999999999995</v>
+      </c>
       <c r="D195" s="144"/>
       <c r="E195" s="144"/>
       <c r="F195" s="144"/>
@@ -9546,7 +9835,9 @@
         <v>42</v>
       </c>
       <c r="B196" s="38"/>
-      <c r="C196" s="173"/>
+      <c r="C196" s="173" t="s">
+        <v>182</v>
+      </c>
       <c r="D196" s="173"/>
       <c r="E196" s="173"/>
       <c r="F196" s="173"/>
@@ -9677,7 +9968,9 @@
       <c r="A201" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="C201" s="140"/>
+      <c r="C201" s="140">
+        <v>685</v>
+      </c>
       <c r="D201" s="140"/>
       <c r="E201" s="140"/>
       <c r="F201" s="140"/>
@@ -9692,7 +9985,9 @@
       <c r="A202" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="C202" s="140"/>
+      <c r="C202" s="140">
+        <v>120.7</v>
+      </c>
       <c r="D202" s="144"/>
       <c r="E202" s="144"/>
       <c r="F202" s="144"/>
@@ -9707,7 +10002,9 @@
       <c r="A203" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="C203" s="140"/>
+      <c r="C203" s="140">
+        <v>70.400000000000006</v>
+      </c>
       <c r="D203" s="144"/>
       <c r="E203" s="144"/>
       <c r="F203" s="144"/>
@@ -9722,7 +10019,9 @@
       <c r="A204" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="C204" s="144"/>
+      <c r="C204" s="195">
+        <v>0.65</v>
+      </c>
       <c r="D204" s="144"/>
       <c r="E204" s="144"/>
       <c r="F204" s="144"/>
@@ -9738,8 +10037,9 @@
         <v>42</v>
       </c>
       <c r="B205" s="38"/>
-      <c r="C205" s="173"/>
-      <c r="D205" s="173"/>
+      <c r="C205" s="173" t="s">
+        <v>182</v>
+      </c>
       <c r="E205" s="173"/>
       <c r="F205" s="173"/>
       <c r="G205" s="173"/>
@@ -9826,7 +10126,9 @@
         <v>27</v>
       </c>
       <c r="B209" s="36"/>
-      <c r="C209" s="144"/>
+      <c r="C209" s="196">
+        <v>0.15</v>
+      </c>
       <c r="D209" s="144"/>
       <c r="E209" s="144"/>
       <c r="F209" s="144"/>
@@ -9846,7 +10148,9 @@
         <v>42</v>
       </c>
       <c r="B210" s="38"/>
-      <c r="C210" s="173"/>
+      <c r="C210" s="173" t="s">
+        <v>182</v>
+      </c>
       <c r="D210" s="173"/>
       <c r="E210" s="173"/>
       <c r="F210" s="173"/>
@@ -10320,7 +10624,7 @@
       <c r="B223" s="38"/>
       <c r="C223" s="177">
         <f t="shared" ref="C223:E226" si="109">C162*C$217+C183*C$218+C192*C$219</f>
-        <v>0</v>
+        <v>597.29452054794524</v>
       </c>
       <c r="D223" s="177">
         <f t="shared" si="109"/>
@@ -10366,7 +10670,7 @@
       <c r="B224" s="38"/>
       <c r="C224" s="177">
         <f t="shared" si="109"/>
-        <v>0</v>
+        <v>70.92328767123287</v>
       </c>
       <c r="D224" s="177">
         <f t="shared" si="109"/>
@@ -10412,7 +10716,7 @@
       <c r="B225" s="38"/>
       <c r="C225" s="177">
         <f t="shared" si="109"/>
-        <v>0</v>
+        <v>49.270410958904108</v>
       </c>
       <c r="D225" s="177">
         <f t="shared" si="109"/>
@@ -10458,7 +10762,7 @@
       <c r="B226" s="38"/>
       <c r="C226" s="178">
         <f t="shared" si="109"/>
-        <v>0</v>
+        <v>0.42619178082191778</v>
       </c>
       <c r="D226" s="178">
         <f t="shared" si="109"/>
@@ -10610,7 +10914,7 @@
       <c r="B230" s="38"/>
       <c r="C230" s="177">
         <f>C183*C$217+C192*C$218+C201*C$219</f>
-        <v>0</v>
+        <v>674.09041095890416</v>
       </c>
       <c r="D230" s="177">
         <f t="shared" ref="D230:L230" si="113">D183*D$217+D192*D$218+D201*D$219</f>
@@ -10656,7 +10960,7 @@
       <c r="B231" s="38"/>
       <c r="C231" s="177">
         <f t="shared" ref="C231:L233" si="114">C184*C$217+C193*C$218+C202*C$219</f>
-        <v>0</v>
+        <v>103.39342465753424</v>
       </c>
       <c r="D231" s="177">
         <f t="shared" si="114"/>
@@ -10702,7 +11006,7 @@
       <c r="B232" s="38"/>
       <c r="C232" s="177">
         <f t="shared" si="114"/>
-        <v>0</v>
+        <v>67.127123287671225</v>
       </c>
       <c r="D232" s="177">
         <f t="shared" si="114"/>
@@ -10748,7 +11052,7 @@
       <c r="B233" s="38"/>
       <c r="C233" s="178">
         <f t="shared" si="114"/>
-        <v>0</v>
+        <v>0.61032876712328754</v>
       </c>
       <c r="D233" s="178">
         <f t="shared" si="114"/>
@@ -10948,7 +11252,7 @@
       </c>
       <c r="C240" s="181">
         <f t="shared" ref="C240:L240" si="117">C53</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="D240" s="181">
         <f t="shared" si="117"/>
@@ -10999,7 +11303,7 @@
       <c r="B241" s="41"/>
       <c r="C241" s="149">
         <f t="shared" ref="C241:L241" si="118">C53*C11</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="D241" s="149">
         <f t="shared" si="118"/>
@@ -11069,7 +11373,7 @@
       <c r="B243" s="24"/>
       <c r="C243" s="181">
         <f t="shared" ref="C243:L243" si="119">C176</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="D243" s="181">
         <f t="shared" si="119"/>
@@ -11120,7 +11424,7 @@
       <c r="B244" s="9"/>
       <c r="C244" s="184">
         <f t="shared" ref="C244:L244" si="120">C241+C176</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="D244" s="184">
         <f t="shared" si="120"/>
@@ -11260,9 +11564,9 @@
       <c r="A249" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C249" s="186" t="str">
+      <c r="C249" s="186">
         <f t="shared" ref="C249:L249" si="122">IFERROR(C244/C154, "NM")</f>
-        <v>NM</v>
+        <v>1.4283414474164087</v>
       </c>
       <c r="D249" s="186" t="str">
         <f t="shared" si="122"/>
@@ -11305,9 +11609,9 @@
       <c r="A250" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C250" s="186" t="str">
+      <c r="C250" s="186">
         <f t="shared" ref="C250:L250" si="123">IFERROR(C244/C155, "NM")</f>
-        <v>NM</v>
+        <v>13.305127464895083</v>
       </c>
       <c r="D250" s="186" t="str">
         <f t="shared" si="123"/>
@@ -11350,9 +11654,9 @@
       <c r="A251" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C251" s="186" t="str">
+      <c r="C251" s="186">
         <f t="shared" ref="C251:L251" si="124">IFERROR(C244/C156, "NM")</f>
-        <v>NM</v>
+        <v>16.454598381675616</v>
       </c>
       <c r="D251" s="186" t="str">
         <f t="shared" si="124"/>
@@ -11395,9 +11699,9 @@
       <c r="A252" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C252" s="186" t="str">
+      <c r="C252" s="186">
         <f t="shared" ref="C252:L252" si="125">IFERROR(C11/C157, "NM")</f>
-        <v>NM</v>
+        <v>18.178824117787183</v>
       </c>
       <c r="D252" s="186" t="str">
         <f t="shared" si="125"/>
@@ -11455,9 +11759,9 @@
       <c r="A254" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C254" s="186" t="str">
+      <c r="C254" s="186">
         <f t="shared" ref="C254:L254" si="126">IFERROR(C$244/C223, "NM")</f>
-        <v>NM</v>
+        <v>0.88519003106702576</v>
       </c>
       <c r="D254" s="186" t="str">
         <f t="shared" si="126"/>
@@ -11500,9 +11804,9 @@
       <c r="A255" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C255" s="186" t="str">
+      <c r="C255" s="186">
         <f t="shared" ref="C255:L255" si="127">IFERROR(C$244/C224, "NM")</f>
-        <v>NM</v>
+        <v>7.454803246726156</v>
       </c>
       <c r="D255" s="186" t="str">
         <f t="shared" si="127"/>
@@ -11545,9 +11849,9 @@
       <c r="A256" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C256" s="186" t="str">
+      <c r="C256" s="186">
         <f t="shared" ref="C256:L256" si="128">IFERROR(C$244/C225, "NM")</f>
-        <v>NM</v>
+        <v>10.730967022803982</v>
       </c>
       <c r="D256" s="186" t="str">
         <f t="shared" si="128"/>
@@ -11590,9 +11894,9 @@
       <c r="A257" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C257" s="186" t="str">
+      <c r="C257" s="186">
         <f t="shared" ref="C257:L257" si="129">IFERROR(C239/C226, "NM")</f>
-        <v>NM</v>
+        <v>13.045770120853691</v>
       </c>
       <c r="D257" s="186" t="str">
         <f t="shared" si="129"/>
@@ -11650,9 +11954,9 @@
       <c r="A259" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C259" s="186" t="str">
+      <c r="C259" s="186">
         <f t="shared" ref="C259:L259" si="130">IFERROR(C$244/C230, "NM")</f>
-        <v>NM</v>
+        <v>0.7843445724852971</v>
       </c>
       <c r="D259" s="186" t="str">
         <f t="shared" si="130"/>
@@ -11695,9 +11999,9 @@
       <c r="A260" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C260" s="186" t="str">
+      <c r="C260" s="186">
         <f t="shared" ref="C260:L260" si="131">IFERROR(C$244/C231, "NM")</f>
-        <v>NM</v>
+        <v>5.1136632426216124</v>
       </c>
       <c r="D260" s="186" t="str">
         <f t="shared" si="131"/>
@@ -11740,9 +12044,9 @@
       <c r="A261" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C261" s="186" t="str">
+      <c r="C261" s="186">
         <f t="shared" ref="C261:L261" si="132">IFERROR(C$244/C232, "NM")</f>
-        <v>NM</v>
+        <v>7.8763863145779425</v>
       </c>
       <c r="D261" s="186" t="str">
         <f t="shared" si="132"/>
@@ -11785,9 +12089,9 @@
       <c r="A262" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C262" s="186" t="str">
+      <c r="C262" s="186">
         <f t="shared" ref="C262:L262" si="133">IFERROR(C239/C233, "NM")</f>
-        <v>NM</v>
+        <v>9.1098442339632815</v>
       </c>
       <c r="D262" s="186" t="str">
         <f t="shared" si="133"/>
@@ -11842,9 +12146,9 @@
       <c r="A264" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C264" s="186" t="str">
+      <c r="C264" s="186">
         <f t="shared" ref="C264:L264" si="134">IFERROR(C257/(C209*100), "NM")</f>
-        <v>NM</v>
+        <v>0.86971800805691268</v>
       </c>
       <c r="D264" s="186" t="str">
         <f t="shared" si="134"/>
@@ -11931,6 +12235,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -12250,75 +12555,75 @@
       </c>
       <c r="C9" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(C$2,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="D9" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(D$2,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="E9" s="83"/>
       <c r="F9" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(F$2,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>0</v>
+        <v>370.1629999999999</v>
       </c>
       <c r="G9" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(G$2,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>0</v>
+        <v>39.737999999999936</v>
       </c>
       <c r="H9" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(H$2,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>0</v>
+        <v>32.131999999999941</v>
       </c>
       <c r="I9" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(I$2,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>0</v>
+        <v>0.3058503654567945</v>
       </c>
       <c r="J9" s="83"/>
       <c r="K9" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(K$2,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>0</v>
+        <v>597.29452054794524</v>
       </c>
       <c r="L9" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(L$2,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>0</v>
+        <v>70.92328767123287</v>
       </c>
       <c r="M9" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(M$2,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>0</v>
+        <v>49.270410958904108</v>
       </c>
       <c r="N9" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(N$2,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>0</v>
+        <v>0.42619178082191778</v>
       </c>
       <c r="O9" s="83"/>
       <c r="P9" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(P$2,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>0</v>
+        <v>674.09041095890416</v>
       </c>
       <c r="Q9" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(Q$2,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>0</v>
+        <v>103.39342465753424</v>
       </c>
       <c r="R9" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(R$2,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>0</v>
+        <v>67.127123287671225</v>
       </c>
       <c r="S9" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(S$2,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>0</v>
+        <v>0.61032876712328754</v>
       </c>
       <c r="T9" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(T$2,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="U9" s="83"/>
       <c r="V9" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(V$2,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="W9" s="85">
         <f>IF(ISBLANK($A9),"",VLOOKUP(W$2,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
     </row>
     <row r="10" spans="1:23">
@@ -13235,59 +13540,59 @@
       <c r="C23" s="84"/>
       <c r="D23" s="89"/>
       <c r="E23" s="90"/>
-      <c r="F23" s="83" t="str">
+      <c r="F23" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(F$3,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>NM</v>
-      </c>
-      <c r="G23" s="83" t="str">
+        <v>1.4283414474164087</v>
+      </c>
+      <c r="G23" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(G$3,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>NM</v>
-      </c>
-      <c r="H23" s="83" t="str">
+        <v>13.305127464895083</v>
+      </c>
+      <c r="H23" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(H$3,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>NM</v>
-      </c>
-      <c r="I23" s="83" t="str">
+        <v>16.454598381675616</v>
+      </c>
+      <c r="I23" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(I$3,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>NM</v>
+        <v>18.178824117787183</v>
       </c>
       <c r="J23" s="83"/>
-      <c r="K23" s="83" t="str">
+      <c r="K23" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(K$3,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>NM</v>
-      </c>
-      <c r="L23" s="83" t="str">
+        <v>0.88519003106702576</v>
+      </c>
+      <c r="L23" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(L$3,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>NM</v>
-      </c>
-      <c r="M23" s="83" t="str">
+        <v>7.454803246726156</v>
+      </c>
+      <c r="M23" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(M$3,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>NM</v>
-      </c>
-      <c r="N23" s="83" t="str">
+        <v>10.730967022803982</v>
+      </c>
+      <c r="N23" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(N$3,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>NM</v>
+        <v>13.045770120853691</v>
       </c>
       <c r="O23" s="83"/>
-      <c r="P23" s="83" t="str">
+      <c r="P23" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(P$3,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>NM</v>
-      </c>
-      <c r="Q23" s="83" t="str">
+        <v>0.7843445724852971</v>
+      </c>
+      <c r="Q23" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(Q$3,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>NM</v>
-      </c>
-      <c r="R23" s="83" t="str">
+        <v>5.1136632426216124</v>
+      </c>
+      <c r="R23" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(R$3,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>NM</v>
-      </c>
-      <c r="S23" s="83" t="str">
+        <v>7.8763863145779425</v>
+      </c>
+      <c r="S23" s="83">
         <f>IF(ISBLANK($A9),"",VLOOKUP(S$3,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>NM</v>
-      </c>
-      <c r="T23" s="85" t="str">
+        <v>9.1098442339632815</v>
+      </c>
+      <c r="T23" s="85">
         <f>IF(ISBLANK($A9),"",VLOOKUP(T$3,Input!$A$6:$L$300,MATCH($A9,Input!$B$6:$L$6,0)+1,FALSE))</f>
-        <v>NM</v>
+        <v>0.86971800805691268</v>
       </c>
       <c r="U23" s="16"/>
       <c r="V23" s="16"/>
@@ -13932,57 +14237,57 @@
       <c r="E34" s="47"/>
       <c r="F34" s="47">
         <f t="shared" ref="F34:T34" si="1">MAX(F23:F32)</f>
-        <v>0</v>
+        <v>1.4283414474164087</v>
       </c>
       <c r="G34" s="47">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>13.305127464895083</v>
       </c>
       <c r="H34" s="47">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>16.454598381675616</v>
       </c>
       <c r="I34" s="47">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>18.178824117787183</v>
       </c>
       <c r="J34" s="47"/>
       <c r="K34" s="47">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.88519003106702576</v>
       </c>
       <c r="L34" s="47">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7.454803246726156</v>
       </c>
       <c r="M34" s="47">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10.730967022803982</v>
       </c>
       <c r="N34" s="47">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>13.045770120853691</v>
       </c>
       <c r="O34" s="47"/>
       <c r="P34" s="47">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.7843445724852971</v>
       </c>
       <c r="Q34" s="47">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5.1136632426216124</v>
       </c>
       <c r="R34" s="47">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7.8763863145779425</v>
       </c>
       <c r="S34" s="47">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9.1098442339632815</v>
       </c>
       <c r="T34" s="47">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.86971800805691268</v>
       </c>
       <c r="U34" s="47"/>
     </row>
@@ -13994,57 +14299,57 @@
       <c r="E35" s="47"/>
       <c r="F35" s="66">
         <f t="shared" ref="F35:T35" si="2">MIN(F23:F32)</f>
-        <v>0</v>
+        <v>1.4283414474164087</v>
       </c>
       <c r="G35" s="66">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>13.305127464895083</v>
       </c>
       <c r="H35" s="66">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16.454598381675616</v>
       </c>
       <c r="I35" s="66">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>18.178824117787183</v>
       </c>
       <c r="J35" s="66"/>
       <c r="K35" s="66">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.88519003106702576</v>
       </c>
       <c r="L35" s="66">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7.454803246726156</v>
       </c>
       <c r="M35" s="66">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10.730967022803982</v>
       </c>
       <c r="N35" s="66">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>13.045770120853691</v>
       </c>
       <c r="O35" s="66"/>
       <c r="P35" s="66">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.7843445724852971</v>
       </c>
       <c r="Q35" s="66">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.1136632426216124</v>
       </c>
       <c r="R35" s="66">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7.8763863145779425</v>
       </c>
       <c r="S35" s="66">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.1098442339632815</v>
       </c>
       <c r="T35" s="66">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.86971800805691268</v>
       </c>
       <c r="U35" s="66"/>
     </row>
@@ -14054,59 +14359,59 @@
       </c>
       <c r="D36" s="47"/>
       <c r="E36" s="47"/>
-      <c r="F36" s="66" t="e">
+      <c r="F36" s="66">
         <f>MEDIAN(F23:F32)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G36" s="66" t="e">
+        <v>1.4283414474164087</v>
+      </c>
+      <c r="G36" s="66">
         <f t="shared" ref="G36:T36" si="3">MEDIAN(G23:G32)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H36" s="66" t="e">
+        <v>13.305127464895083</v>
+      </c>
+      <c r="H36" s="66">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="I36" s="66" t="e">
+        <v>16.454598381675616</v>
+      </c>
+      <c r="I36" s="66">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>18.178824117787183</v>
       </c>
       <c r="J36" s="66"/>
-      <c r="K36" s="66" t="e">
+      <c r="K36" s="66">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="L36" s="66" t="e">
+        <v>0.88519003106702576</v>
+      </c>
+      <c r="L36" s="66">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="M36" s="66" t="e">
+        <v>7.454803246726156</v>
+      </c>
+      <c r="M36" s="66">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N36" s="66" t="e">
+        <v>10.730967022803982</v>
+      </c>
+      <c r="N36" s="66">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>13.045770120853691</v>
       </c>
       <c r="O36" s="66"/>
-      <c r="P36" s="66" t="e">
+      <c r="P36" s="66">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="Q36" s="66" t="e">
+        <v>0.7843445724852971</v>
+      </c>
+      <c r="Q36" s="66">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="R36" s="66" t="e">
+        <v>5.1136632426216124</v>
+      </c>
+      <c r="R36" s="66">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="S36" s="66" t="e">
+        <v>7.8763863145779425</v>
+      </c>
+      <c r="S36" s="66">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T36" s="66" t="e">
+        <v>9.1098442339632815</v>
+      </c>
+      <c r="T36" s="66">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>0.86971800805691268</v>
       </c>
       <c r="U36" s="66"/>
     </row>
@@ -14116,59 +14421,59 @@
       </c>
       <c r="D37" s="47"/>
       <c r="E37" s="47"/>
-      <c r="F37" s="67" t="e">
+      <c r="F37" s="67">
         <f>AVERAGE(F23:F32)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G37" s="67" t="e">
+        <v>1.4283414474164087</v>
+      </c>
+      <c r="G37" s="67">
         <f t="shared" ref="G37:T37" si="4">AVERAGE(G23:G32)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H37" s="67" t="e">
+        <v>13.305127464895083</v>
+      </c>
+      <c r="H37" s="67">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I37" s="67" t="e">
+        <v>16.454598381675616</v>
+      </c>
+      <c r="I37" s="67">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>18.178824117787183</v>
       </c>
       <c r="J37" s="67"/>
-      <c r="K37" s="67" t="e">
+      <c r="K37" s="67">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L37" s="67" t="e">
+        <v>0.88519003106702576</v>
+      </c>
+      <c r="L37" s="67">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M37" s="67" t="e">
+        <v>7.454803246726156</v>
+      </c>
+      <c r="M37" s="67">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N37" s="67" t="e">
+        <v>10.730967022803982</v>
+      </c>
+      <c r="N37" s="67">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>13.045770120853691</v>
       </c>
       <c r="O37" s="67"/>
-      <c r="P37" s="67" t="e">
+      <c r="P37" s="67">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q37" s="67" t="e">
+        <v>0.7843445724852971</v>
+      </c>
+      <c r="Q37" s="67">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R37" s="67" t="e">
+        <v>5.1136632426216124</v>
+      </c>
+      <c r="R37" s="67">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S37" s="67" t="e">
+        <v>7.8763863145779425</v>
+      </c>
+      <c r="S37" s="67">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T37" s="67" t="e">
+        <v>9.1098442339632815</v>
+      </c>
+      <c r="T37" s="67">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.86971800805691268</v>
       </c>
       <c r="U37" s="67"/>
     </row>
@@ -14242,59 +14547,59 @@
       </c>
       <c r="D39" s="47"/>
       <c r="E39" s="47"/>
-      <c r="F39" s="67" t="str">
+      <c r="F39" s="67">
         <f>F23</f>
-        <v>NM</v>
-      </c>
-      <c r="G39" s="67" t="str">
+        <v>1.4283414474164087</v>
+      </c>
+      <c r="G39" s="67">
         <f t="shared" ref="G39:T39" si="5">G23</f>
-        <v>NM</v>
-      </c>
-      <c r="H39" s="67" t="str">
+        <v>13.305127464895083</v>
+      </c>
+      <c r="H39" s="67">
         <f t="shared" si="5"/>
-        <v>NM</v>
-      </c>
-      <c r="I39" s="67" t="str">
+        <v>16.454598381675616</v>
+      </c>
+      <c r="I39" s="67">
         <f t="shared" si="5"/>
-        <v>NM</v>
+        <v>18.178824117787183</v>
       </c>
       <c r="J39" s="67"/>
-      <c r="K39" s="67" t="str">
+      <c r="K39" s="67">
         <f t="shared" si="5"/>
-        <v>NM</v>
-      </c>
-      <c r="L39" s="67" t="str">
+        <v>0.88519003106702576</v>
+      </c>
+      <c r="L39" s="67">
         <f t="shared" si="5"/>
-        <v>NM</v>
-      </c>
-      <c r="M39" s="67" t="str">
+        <v>7.454803246726156</v>
+      </c>
+      <c r="M39" s="67">
         <f t="shared" si="5"/>
-        <v>NM</v>
-      </c>
-      <c r="N39" s="67" t="str">
+        <v>10.730967022803982</v>
+      </c>
+      <c r="N39" s="67">
         <f t="shared" si="5"/>
-        <v>NM</v>
+        <v>13.045770120853691</v>
       </c>
       <c r="O39" s="67"/>
-      <c r="P39" s="67" t="str">
+      <c r="P39" s="67">
         <f t="shared" si="5"/>
-        <v>NM</v>
-      </c>
-      <c r="Q39" s="67" t="str">
+        <v>0.7843445724852971</v>
+      </c>
+      <c r="Q39" s="67">
         <f t="shared" si="5"/>
-        <v>NM</v>
-      </c>
-      <c r="R39" s="67" t="str">
+        <v>5.1136632426216124</v>
+      </c>
+      <c r="R39" s="67">
         <f t="shared" si="5"/>
-        <v>NM</v>
-      </c>
-      <c r="S39" s="67" t="str">
+        <v>7.8763863145779425</v>
+      </c>
+      <c r="S39" s="67">
         <f t="shared" si="5"/>
-        <v>NM</v>
-      </c>
-      <c r="T39" s="67" t="str">
+        <v>9.1098442339632815</v>
+      </c>
+      <c r="T39" s="67">
         <f t="shared" si="5"/>
-        <v>NM</v>
+        <v>0.86971800805691268</v>
       </c>
       <c r="U39" s="67"/>
     </row>
@@ -14466,59 +14771,59 @@
         <f>Output!C36</f>
         <v>Median</v>
       </c>
-      <c r="B6" s="105" t="e">
+      <c r="B6" s="105">
         <f>Output!F37</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C6" s="105" t="e">
+        <v>1.4283414474164087</v>
+      </c>
+      <c r="C6" s="105">
         <f>Output!G37</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D6" s="105" t="e">
+        <v>13.305127464895083</v>
+      </c>
+      <c r="D6" s="105">
         <f>Output!H37</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E6" s="105" t="e">
+        <v>16.454598381675616</v>
+      </c>
+      <c r="E6" s="105">
         <f>Output!I37</f>
-        <v>#DIV/0!</v>
+        <v>18.178824117787183</v>
       </c>
       <c r="F6" s="105"/>
-      <c r="G6" s="105" t="e">
+      <c r="G6" s="105">
         <f>Output!K37</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H6" s="105" t="e">
+        <v>0.88519003106702576</v>
+      </c>
+      <c r="H6" s="105">
         <f>Output!L37</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I6" s="105" t="e">
+        <v>7.454803246726156</v>
+      </c>
+      <c r="I6" s="105">
         <f>Output!M37</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J6" s="105" t="e">
+        <v>10.730967022803982</v>
+      </c>
+      <c r="J6" s="105">
         <f>Output!N37</f>
-        <v>#DIV/0!</v>
+        <v>13.045770120853691</v>
       </c>
       <c r="K6" s="105"/>
-      <c r="L6" s="105" t="e">
+      <c r="L6" s="105">
         <f>Output!P37</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M6" s="105" t="e">
+        <v>0.7843445724852971</v>
+      </c>
+      <c r="M6" s="105">
         <f>Output!Q37</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N6" s="105" t="e">
+        <v>5.1136632426216124</v>
+      </c>
+      <c r="N6" s="105">
         <f>Output!R37</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O6" s="105" t="e">
+        <v>7.8763863145779425</v>
+      </c>
+      <c r="O6" s="105">
         <f>Output!S37</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P6" s="105" t="e">
+        <v>9.1098442339632815</v>
+      </c>
+      <c r="P6" s="105">
         <f>Output!T37</f>
-        <v>#DIV/0!</v>
+        <v>0.86971800805691268</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -14527,57 +14832,57 @@
       </c>
       <c r="B7" s="107">
         <f>Output!F34</f>
-        <v>0</v>
+        <v>1.4283414474164087</v>
       </c>
       <c r="C7" s="107">
         <f>Output!G34</f>
-        <v>0</v>
+        <v>13.305127464895083</v>
       </c>
       <c r="D7" s="107">
         <f>Output!H34</f>
-        <v>0</v>
+        <v>16.454598381675616</v>
       </c>
       <c r="E7" s="107">
         <f>Output!I34</f>
-        <v>0</v>
+        <v>18.178824117787183</v>
       </c>
       <c r="F7" s="107"/>
       <c r="G7" s="107">
         <f>Output!K34</f>
-        <v>0</v>
+        <v>0.88519003106702576</v>
       </c>
       <c r="H7" s="107">
         <f>Output!L34</f>
-        <v>0</v>
+        <v>7.454803246726156</v>
       </c>
       <c r="I7" s="107">
         <f>Output!M34</f>
-        <v>0</v>
+        <v>10.730967022803982</v>
       </c>
       <c r="J7" s="107">
         <f>Output!N34</f>
-        <v>0</v>
+        <v>13.045770120853691</v>
       </c>
       <c r="K7" s="107"/>
       <c r="L7" s="107">
         <f>Output!P34</f>
-        <v>0</v>
+        <v>0.7843445724852971</v>
       </c>
       <c r="M7" s="107">
         <f>Output!Q34</f>
-        <v>0</v>
+        <v>5.1136632426216124</v>
       </c>
       <c r="N7" s="107">
         <f>Output!R34</f>
-        <v>0</v>
+        <v>7.8763863145779425</v>
       </c>
       <c r="O7" s="107">
         <f>Output!S34</f>
-        <v>0</v>
+        <v>9.1098442339632815</v>
       </c>
       <c r="P7" s="107">
         <f>Output!T34</f>
-        <v>0</v>
+        <v>0.86971800805691268</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -14586,57 +14891,57 @@
       </c>
       <c r="B8" s="107">
         <f>Output!F35</f>
-        <v>0</v>
+        <v>1.4283414474164087</v>
       </c>
       <c r="C8" s="107">
         <f>Output!G35</f>
-        <v>0</v>
+        <v>13.305127464895083</v>
       </c>
       <c r="D8" s="107">
         <f>Output!H35</f>
-        <v>0</v>
+        <v>16.454598381675616</v>
       </c>
       <c r="E8" s="107">
         <f>Output!I35</f>
-        <v>0</v>
+        <v>18.178824117787183</v>
       </c>
       <c r="F8" s="107"/>
       <c r="G8" s="107">
         <f>Output!K35</f>
-        <v>0</v>
+        <v>0.88519003106702576</v>
       </c>
       <c r="H8" s="107">
         <f>Output!L35</f>
-        <v>0</v>
+        <v>7.454803246726156</v>
       </c>
       <c r="I8" s="107">
         <f>Output!M35</f>
-        <v>0</v>
+        <v>10.730967022803982</v>
       </c>
       <c r="J8" s="107">
         <f>Output!N35</f>
-        <v>0</v>
+        <v>13.045770120853691</v>
       </c>
       <c r="K8" s="107"/>
       <c r="L8" s="107">
         <f>Output!P35</f>
-        <v>0</v>
+        <v>0.7843445724852971</v>
       </c>
       <c r="M8" s="107">
         <f>Output!Q35</f>
-        <v>0</v>
+        <v>5.1136632426216124</v>
       </c>
       <c r="N8" s="107">
         <f>Output!R35</f>
-        <v>0</v>
+        <v>7.8763863145779425</v>
       </c>
       <c r="O8" s="107">
         <f>Output!S35</f>
-        <v>0</v>
+        <v>9.1098442339632815</v>
       </c>
       <c r="P8" s="107">
         <f>Output!T35</f>
-        <v>0</v>
+        <v>0.86971800805691268</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -14736,57 +15041,57 @@
       <c r="A14" s="97" t="s">
         <v>136</v>
       </c>
-      <c r="B14" s="18" t="e">
+      <c r="B14" s="18">
         <f>B6*Output!F9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C14" s="18" t="e">
+        <v>528.71915519999993</v>
+      </c>
+      <c r="C14" s="18">
         <f>C6*Output!G9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D14" s="18" t="e">
+        <v>528.71915519999993</v>
+      </c>
+      <c r="D14" s="18">
         <f>D6*Output!H9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E14" s="18" t="e">
+        <v>528.71915519999993</v>
+      </c>
+      <c r="E14" s="18">
         <f>E16+E15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G14" s="18" t="e">
+        <v>528.71915519999993</v>
+      </c>
+      <c r="G14" s="18">
         <f>G6*Output!K9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H14" s="18" t="e">
+        <v>528.71915519999993</v>
+      </c>
+      <c r="H14" s="18">
         <f>H6*Output!L9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I14" s="18" t="e">
+        <v>528.71915519999993</v>
+      </c>
+      <c r="I14" s="18">
         <f>I6*Output!M9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J14" s="18" t="e">
+        <v>528.71915519999993</v>
+      </c>
+      <c r="J14" s="18">
         <f>J16+J15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L14" s="18" t="e">
+        <v>528.71915519999993</v>
+      </c>
+      <c r="L14" s="18">
         <f>L6*Output!P9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M14" s="18" t="e">
+        <v>528.71915519999993</v>
+      </c>
+      <c r="M14" s="18">
         <f>M6*Output!Q9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N14" s="18" t="e">
+        <v>528.71915519999993</v>
+      </c>
+      <c r="N14" s="18">
         <f>N6*Output!R9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O14" s="18" t="e">
+        <v>528.71915519999993</v>
+      </c>
+      <c r="O14" s="18">
         <f>O16+O15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P14" s="18" t="e">
+        <v>528.71915519999993</v>
+      </c>
+      <c r="P14" s="18">
         <f>P16+P15</f>
-        <v>#DIV/0!</v>
+        <v>528.71915519999993</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -14795,112 +15100,112 @@
       </c>
       <c r="B15" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="C15" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="D15" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="E15" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="G15" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="H15" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="I15" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="J15" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="L15" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="M15" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="N15" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="O15" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="P15" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="97" t="s">
         <v>135</v>
       </c>
-      <c r="B16" s="94" t="e">
+      <c r="B16" s="94">
         <f>B14-B15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C16" s="94" t="e">
+        <v>541.54815519999988</v>
+      </c>
+      <c r="C16" s="94">
         <f>C14-C15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D16" s="94" t="e">
+        <v>541.54815519999988</v>
+      </c>
+      <c r="D16" s="94">
         <f>D14-D15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E16" s="94" t="e">
+        <v>541.54815519999988</v>
+      </c>
+      <c r="E16" s="94">
         <f>E6*Output!$I$9*Output!$W$9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G16" s="94" t="e">
+        <v>541.54815519999988</v>
+      </c>
+      <c r="G16" s="94">
         <f>G14-G15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H16" s="94" t="e">
+        <v>541.54815519999988</v>
+      </c>
+      <c r="H16" s="94">
         <f>H14-H15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I16" s="94" t="e">
+        <v>541.54815519999988</v>
+      </c>
+      <c r="I16" s="94">
         <f>I14-I15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J16" s="94" t="e">
+        <v>541.54815519999988</v>
+      </c>
+      <c r="J16" s="94">
         <f>J6*Output!N9*Output!$W$9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L16" s="94" t="e">
+        <v>541.54815519999988</v>
+      </c>
+      <c r="L16" s="94">
         <f>L14-L15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M16" s="94" t="e">
+        <v>541.54815519999988</v>
+      </c>
+      <c r="M16" s="94">
         <f>M14-M15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N16" s="94" t="e">
+        <v>541.54815519999988</v>
+      </c>
+      <c r="N16" s="94">
         <f>N14-N15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O16" s="94" t="e">
+        <v>541.54815519999988</v>
+      </c>
+      <c r="O16" s="94">
         <f>O6*Output!S9*Output!$W$9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P16" s="95" t="e">
+        <v>541.54815519999988</v>
+      </c>
+      <c r="P16" s="95">
         <f>100*P6*Output!T$9*Output!N$9*Output!$W$9</f>
-        <v>#DIV/0!</v>
+        <v>541.54815519999988</v>
       </c>
     </row>
     <row r="17" spans="1:22">
@@ -14909,114 +15214,114 @@
       </c>
       <c r="B17" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="C17" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="D17" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="E17" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="G17" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="H17" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="I17" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="J17" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="L17" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="M17" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="N17" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="O17" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="P17" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="98" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="96" t="e">
+      <c r="B18" s="96">
         <f>B16/B17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C18" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="C18" s="96">
         <f>C16/C17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D18" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="D18" s="96">
         <f>D16/D17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E18" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="E18" s="96">
         <f>E16/E17</f>
-        <v>#DIV/0!</v>
+        <v>5.5599999999999987</v>
       </c>
       <c r="F18" s="96"/>
-      <c r="G18" s="96" t="e">
+      <c r="G18" s="96">
         <f>G16/G17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H18" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="H18" s="96">
         <f>H16/H17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I18" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="I18" s="96">
         <f>I16/I17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J18" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="J18" s="96">
         <f>J16/J17</f>
-        <v>#DIV/0!</v>
+        <v>5.5599999999999987</v>
       </c>
       <c r="K18" s="96"/>
-      <c r="L18" s="96" t="e">
+      <c r="L18" s="96">
         <f>L16/L17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M18" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="M18" s="96">
         <f>M16/M17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N18" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="N18" s="96">
         <f>N16/N17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O18" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="O18" s="96">
         <f>O16/O17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P18" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="P18" s="96">
         <f>P16/P17</f>
-        <v>#DIV/0!</v>
+        <v>5.5599999999999987</v>
       </c>
     </row>
     <row r="20" spans="1:22">
@@ -15030,55 +15335,55 @@
       </c>
       <c r="B21" s="18">
         <f>B7*Output!F9</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="C21" s="18">
         <f>C7*Output!G9</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="D21" s="18">
         <f>D7*Output!H9</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="E21" s="18">
         <f>E23+E22</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="G21" s="18">
         <f>G7*Output!K9</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="H21" s="18">
         <f>H7*Output!L9</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="I21" s="18">
         <f>I7*Output!M9</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="J21" s="18">
         <f>J23+J22</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="L21" s="18">
         <f>L7*Output!P9</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="M21" s="18">
         <f>M7*Output!Q9</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="N21" s="18">
         <f>N7*Output!R9</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="O21" s="18">
         <f>O23+O22</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="P21" s="18">
         <f>P23+P22</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
     </row>
     <row r="22" spans="1:22">
@@ -15087,56 +15392,56 @@
       </c>
       <c r="B22" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="C22" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="D22" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="E22" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="F22" s="93"/>
       <c r="G22" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="H22" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="I22" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="J22" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="L22" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="M22" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="N22" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="O22" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="P22" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
     </row>
     <row r="23" spans="1:22">
@@ -15145,55 +15450,55 @@
       </c>
       <c r="B23" s="94">
         <f>B21-B22</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="C23" s="94">
         <f>C21-C22</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="D23" s="94">
         <f>D21-D22</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="E23" s="94">
         <f>E7*Output!$I$9*Output!$W$9</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="G23" s="94">
         <f>G21-G22</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="H23" s="94">
         <f>H21-H22</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="I23" s="94">
         <f>I21-I22</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="J23" s="94">
         <f>J7*Output!$N$9*Output!$W$9</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="L23" s="94">
         <f>L21-L22</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="M23" s="94">
         <f>M21-M22</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="N23" s="94">
         <f>N21-N22</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="O23" s="94">
         <f>O7*Output!S9*Output!$W$9</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="P23" s="95">
         <f>100*P7*Output!T$9*Output!N$9*Output!$W$9</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
     </row>
     <row r="24" spans="1:22">
@@ -15202,114 +15507,114 @@
       </c>
       <c r="B24" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="C24" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="D24" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="E24" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="G24" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="H24" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="I24" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="J24" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="L24" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="M24" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="N24" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="O24" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="P24" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="98" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="96" t="e">
+      <c r="B25" s="96">
         <f>B23/B24</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C25" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="C25" s="96">
         <f>C23/C24</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D25" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="D25" s="96">
         <f>D23/D24</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E25" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="E25" s="96">
         <f>E23/E24</f>
-        <v>#DIV/0!</v>
+        <v>5.5599999999999987</v>
       </c>
       <c r="F25" s="96"/>
-      <c r="G25" s="96" t="e">
+      <c r="G25" s="96">
         <f>G23/G24</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H25" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="H25" s="96">
         <f>H23/H24</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I25" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="I25" s="96">
         <f>I23/I24</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J25" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="J25" s="96">
         <f>J23/J24</f>
-        <v>#DIV/0!</v>
+        <v>5.5599999999999987</v>
       </c>
       <c r="K25" s="96"/>
-      <c r="L25" s="96" t="e">
+      <c r="L25" s="96">
         <f>L23/L24</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M25" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="M25" s="96">
         <f>M23/M24</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N25" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="N25" s="96">
         <f>N23/N24</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O25" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="O25" s="96">
         <f>O23/O24</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P25" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="P25" s="96">
         <f>P23/P24</f>
-        <v>#DIV/0!</v>
+        <v>5.5599999999999987</v>
       </c>
     </row>
     <row r="26" spans="1:22">
@@ -15326,55 +15631,55 @@
       </c>
       <c r="B28" s="18">
         <f>B8*Output!F9</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="C28" s="18">
         <f>C8*Output!G9</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="D28" s="18">
         <f>D8*Output!H9</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="E28" s="18">
         <f>E30+E29</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="G28" s="18">
         <f>G8*Output!K9</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="H28" s="18">
         <f>H8*Output!L9</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="I28" s="18">
         <f>I8*Output!M9</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="J28" s="18">
         <f>J30+J29</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="L28" s="18">
         <f>L8*Output!P9</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="M28" s="18">
         <f>M8*Output!Q9</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="N28" s="18">
         <f>N8*Output!R9</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="O28" s="18">
         <f>O30+O29</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
       <c r="P28" s="18">
         <f>P30+P29</f>
-        <v>0</v>
+        <v>528.71915519999993</v>
       </c>
     </row>
     <row r="29" spans="1:22">
@@ -15383,55 +15688,55 @@
       </c>
       <c r="B29" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="C29" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="D29" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="E29" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="G29" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="H29" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="I29" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="J29" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="L29" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="M29" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="N29" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="O29" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
       <c r="P29" s="93">
         <f>Output!$V$9</f>
-        <v>0</v>
+        <v>-12.828999999999994</v>
       </c>
     </row>
     <row r="30" spans="1:22">
@@ -15440,55 +15745,55 @@
       </c>
       <c r="B30" s="94">
         <f>B28-B29</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="C30" s="94">
         <f>C28-C29</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="D30" s="94">
         <f>D28-D29</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="E30" s="94">
         <f>E8*Output!$I$9*Output!$W$9</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="G30" s="18">
         <f>G28-G29</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="H30" s="18">
         <f>H28-H29</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="I30" s="18">
         <f>I28-I29</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="J30" s="94">
         <f>J8*Output!N9*Output!$W$9</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="L30" s="18">
         <f>L28-L29</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="M30" s="18">
         <f>M28-M29</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="N30" s="18">
         <f>N28-N29</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="O30" s="94">
         <f>O8*Output!S9*Output!$W$9</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
       <c r="P30" s="95">
         <f>100*P8*Output!T$9*Output!N$9*Output!$W$9</f>
-        <v>0</v>
+        <v>541.54815519999988</v>
       </c>
     </row>
     <row r="31" spans="1:22">
@@ -15497,114 +15802,114 @@
       </c>
       <c r="B31" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="C31" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="D31" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="E31" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="G31" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="H31" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="I31" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="J31" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="L31" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="M31" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="N31" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="O31" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
       <c r="P31" s="93">
         <f>Output!$W$9</f>
-        <v>0</v>
+        <v>97.400747338129491</v>
       </c>
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="98" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="96" t="e">
+      <c r="B32" s="96">
         <f>B30/B31</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C32" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="C32" s="96">
         <f>C30/C31</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D32" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="D32" s="96">
         <f>D30/D31</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E32" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="E32" s="96">
         <f>E30/E31</f>
-        <v>#DIV/0!</v>
+        <v>5.5599999999999987</v>
       </c>
       <c r="F32" s="96"/>
-      <c r="G32" s="96" t="e">
+      <c r="G32" s="96">
         <f>G30/G31</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H32" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="H32" s="96">
         <f>H30/H31</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I32" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="I32" s="96">
         <f>I30/I31</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J32" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="J32" s="96">
         <f>J30/J31</f>
-        <v>#DIV/0!</v>
+        <v>5.5599999999999987</v>
       </c>
       <c r="K32" s="96"/>
-      <c r="L32" s="96" t="e">
+      <c r="L32" s="96">
         <f>L30/L31</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M32" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="M32" s="96">
         <f>M30/M31</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N32" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="N32" s="96">
         <f>N30/N31</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O32" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="O32" s="96">
         <f>O30/O31</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P32" s="96" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="P32" s="96">
         <f>P30/P31</f>
-        <v>#DIV/0!</v>
+        <v>5.5599999999999987</v>
       </c>
     </row>
   </sheetData>
@@ -15645,17 +15950,17 @@
       <c r="A2" s="112" t="s">
         <v>180</v>
       </c>
-      <c r="B2" s="137" t="e">
+      <c r="B2" s="137">
         <f>'Valuation Matrix'!I32</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C2" s="110" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="C2" s="110">
         <f t="shared" ref="C2:C7" si="0">D2-B2</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D2" s="137" t="e">
+        <v>0</v>
+      </c>
+      <c r="D2" s="137">
         <f>'Valuation Matrix'!I25</f>
-        <v>#DIV/0!</v>
+        <v>5.5599999999999987</v>
       </c>
       <c r="G2" s="109"/>
     </row>
@@ -15663,17 +15968,17 @@
       <c r="A3" s="112" t="s">
         <v>143</v>
       </c>
-      <c r="B3" s="138" t="e">
+      <c r="B3" s="138">
         <f>'Valuation Matrix'!C32</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C3" s="110" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="C3" s="110">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D3" s="138" t="e">
+        <v>0</v>
+      </c>
+      <c r="D3" s="138">
         <f>'Valuation Matrix'!C25</f>
-        <v>#DIV/0!</v>
+        <v>5.5599999999999987</v>
       </c>
       <c r="G3" s="109"/>
     </row>
@@ -15681,17 +15986,17 @@
       <c r="A4" s="112" t="s">
         <v>144</v>
       </c>
-      <c r="B4" s="138" t="e">
+      <c r="B4" s="138">
         <f>'Valuation Matrix'!D32</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C4" s="110" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="C4" s="110">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D4" s="138" t="e">
+        <v>0</v>
+      </c>
+      <c r="D4" s="138">
         <f>'Valuation Matrix'!D25</f>
-        <v>#DIV/0!</v>
+        <v>5.5599999999999987</v>
       </c>
       <c r="G4" s="109"/>
     </row>
@@ -15699,17 +16004,17 @@
       <c r="A5" s="112" t="s">
         <v>145</v>
       </c>
-      <c r="B5" s="138" t="e">
+      <c r="B5" s="138">
         <f>'Valuation Matrix'!E32</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C5" s="110" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="C5" s="110">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D5" s="138" t="e">
+        <v>0</v>
+      </c>
+      <c r="D5" s="138">
         <f>'Valuation Matrix'!E25</f>
-        <v>#DIV/0!</v>
+        <v>5.5599999999999987</v>
       </c>
       <c r="G5" s="109"/>
     </row>
@@ -15717,17 +16022,17 @@
       <c r="A6" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="B6" s="138" t="e">
+      <c r="B6" s="138">
         <f>'Valuation Matrix'!J32</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C6" s="110" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="C6" s="110">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D6" s="138" t="e">
+        <v>0</v>
+      </c>
+      <c r="D6" s="138">
         <f>'Valuation Matrix'!J25</f>
-        <v>#DIV/0!</v>
+        <v>5.5599999999999987</v>
       </c>
       <c r="G6" s="109"/>
     </row>
@@ -15735,17 +16040,17 @@
       <c r="A7" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="B7" s="138" t="e">
+      <c r="B7" s="138">
         <f>'Valuation Matrix'!P32</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C7" s="110" t="e">
+        <v>5.5599999999999987</v>
+      </c>
+      <c r="C7" s="110">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D7" s="138" t="e">
+        <v>0</v>
+      </c>
+      <c r="D7" s="138">
         <f>'Valuation Matrix'!P25</f>
-        <v>#DIV/0!</v>
+        <v>5.5599999999999987</v>
       </c>
       <c r="G7" s="109"/>
     </row>

</xml_diff>